<commit_message>
Cambio nombre doc proyecto final, actualizacion de contenidos
</commit_message>
<xml_diff>
--- a/doc/cuadros y figuras.xlsx
+++ b/doc/cuadros y figuras.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FDD instancias" sheetId="1" r:id="rId1"/>
     <sheet name="FDD resultados" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="DJD resultados" sheetId="3" r:id="rId3"/>
+    <sheet name="DJD res HH" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="123">
   <si>
     <t>Instancia 1</t>
   </si>
@@ -262,13 +263,136 @@
   </si>
   <si>
     <t>189, 162, 158, 154, 150, 150, 150, 150, 10, 10, 9</t>
+  </si>
+  <si>
+    <t>Instancia</t>
+  </si>
+  <si>
+    <t>DJD 1/4</t>
+  </si>
+  <si>
+    <t>DJD 1/3</t>
+  </si>
+  <si>
+    <t>PF01</t>
+  </si>
+  <si>
+    <t>PF02</t>
+  </si>
+  <si>
+    <t>PF03</t>
+  </si>
+  <si>
+    <t>PF04</t>
+  </si>
+  <si>
+    <t>PF05</t>
+  </si>
+  <si>
+    <t>PF06</t>
+  </si>
+  <si>
+    <t>PF07</t>
+  </si>
+  <si>
+    <t>PF08</t>
+  </si>
+  <si>
+    <t>PF09</t>
+  </si>
+  <si>
+    <t>PF10</t>
+  </si>
+  <si>
+    <t>PF11</t>
+  </si>
+  <si>
+    <t>PF12</t>
+  </si>
+  <si>
+    <t>PF13</t>
+  </si>
+  <si>
+    <t>PF14</t>
+  </si>
+  <si>
+    <t>PF15</t>
+  </si>
+  <si>
+    <t>PF16</t>
+  </si>
+  <si>
+    <t>PF17</t>
+  </si>
+  <si>
+    <t>PF18</t>
+  </si>
+  <si>
+    <t>PF19</t>
+  </si>
+  <si>
+    <t>PF20</t>
+  </si>
+  <si>
+    <t>Cant. de Piezas</t>
+  </si>
+  <si>
+    <t>Cant. Cont.</t>
+  </si>
+  <si>
+    <t>Número teórico de cont.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocupación promedio por pieza en cont.  </t>
+  </si>
+  <si>
+    <t>Cant. Piezas más anchas que C. I.</t>
+  </si>
+  <si>
+    <t>Mejores resultados obtenidos con Capacidad Inicial:</t>
+  </si>
+  <si>
+    <t>Inst.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPC  </t>
+  </si>
+  <si>
+    <t>NTC</t>
+  </si>
+  <si>
+    <t>Conts.</t>
+  </si>
+  <si>
+    <t>CPA</t>
+  </si>
+  <si>
+    <t>Igual</t>
+  </si>
+  <si>
+    <t>Igual Count</t>
+  </si>
+  <si>
+    <t>0.33 Count</t>
+  </si>
+  <si>
+    <t>0.25 Count</t>
+  </si>
+  <si>
+    <t>Grand Count</t>
+  </si>
+  <si>
+    <t>Mejores resultados obtenidos Heurística:</t>
+  </si>
+  <si>
+    <t>Heurística seleccionada por HH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +450,21 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -341,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -444,11 +583,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -523,23 +765,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,34 +1156,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -999,34 +1300,34 @@
       <c r="F9" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -1229,34 +1530,34 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1453,34 +1754,34 @@
       <c r="F37" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
@@ -1656,7 +1957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
@@ -1673,21 +1974,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
@@ -1810,21 +2111,21 @@
       <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -1932,18 +2233,18 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
@@ -2210,18 +2511,18 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
     </row>
     <row r="53" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
@@ -2403,18 +2704,18 @@
       <c r="C69" s="17"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
     </row>
     <row r="72" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
@@ -2505,18 +2806,18 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B81" s="30"/>
-      <c r="C81" s="30"/>
+      <c r="B81" s="31"/>
+      <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
@@ -2619,6 +2920,9 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A81:C81"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
@@ -2630,9 +2934,6 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A71:C71"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A81:C81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2641,188 +2942,1632 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="B1:X51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="10.5" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="37"/>
+    <col min="2" max="2" width="7.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="38" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="37"/>
+    <col min="12" max="12" width="13" style="38" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="37"/>
+    <col min="14" max="14" width="4.42578125" style="37" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="11.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:21" s="35" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="45"/>
+      <c r="H2" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="45"/>
+      <c r="L2" s="36"/>
+      <c r="N2" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="45"/>
+      <c r="T2" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="45"/>
+    </row>
+    <row r="3" spans="2:21" s="35" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="S3" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="T3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="U3" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B4" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="41">
+        <v>8</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="43">
+        <v>4</v>
+      </c>
+      <c r="F4" s="48">
+        <v>4</v>
+      </c>
+      <c r="G4" s="49">
+        <v>2</v>
+      </c>
+      <c r="H4" s="48">
+        <v>4</v>
+      </c>
+      <c r="I4" s="49">
+        <v>2</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="41" t="str">
+        <f>IF(F4&gt;H4,0.33,IF(F4=H4, "Igual", 0.25))</f>
+        <v>Igual</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="41">
+        <v>8</v>
+      </c>
+      <c r="P4" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>4</v>
+      </c>
+      <c r="R4" s="48">
+        <v>4</v>
+      </c>
+      <c r="S4" s="49">
+        <v>2</v>
+      </c>
+      <c r="T4" s="48">
+        <v>4</v>
+      </c>
+      <c r="U4" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B5" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="41">
+        <v>30</v>
+      </c>
+      <c r="D5" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="43">
+        <v>6</v>
+      </c>
+      <c r="F5" s="48">
+        <v>8</v>
+      </c>
+      <c r="G5" s="49">
+        <v>2</v>
+      </c>
+      <c r="H5" s="48">
+        <v>7</v>
+      </c>
+      <c r="I5" s="49">
+        <v>2</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="41">
+        <f t="shared" ref="L5:L23" si="0">IF(F5&gt;H5,0.33,IF(F5=H5, "Igual", 0.25))</f>
+        <v>0.33</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="41">
+        <v>30</v>
+      </c>
+      <c r="P5" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q5" s="43">
+        <v>6</v>
+      </c>
+      <c r="R5" s="48">
+        <v>8</v>
+      </c>
+      <c r="S5" s="49">
+        <v>2</v>
+      </c>
+      <c r="T5" s="48">
+        <v>7</v>
+      </c>
+      <c r="U5" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B6" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="41">
+        <v>28</v>
+      </c>
+      <c r="D6" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="43">
+        <v>7</v>
+      </c>
+      <c r="F6" s="48">
+        <v>8</v>
+      </c>
+      <c r="G6" s="49">
+        <v>0</v>
+      </c>
+      <c r="H6" s="48">
+        <v>8</v>
+      </c>
+      <c r="I6" s="49">
+        <v>0</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="O6" s="41">
+        <v>28</v>
+      </c>
+      <c r="P6" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="Q6" s="43">
+        <v>7</v>
+      </c>
+      <c r="R6" s="48">
+        <v>8</v>
+      </c>
+      <c r="S6" s="49">
+        <v>0</v>
+      </c>
+      <c r="T6" s="48">
+        <v>8</v>
+      </c>
+      <c r="U6" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B7" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="41">
+        <v>36</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E7" s="43">
+        <v>6</v>
+      </c>
+      <c r="F7" s="48">
+        <v>7</v>
+      </c>
+      <c r="G7" s="49">
+        <v>0</v>
+      </c>
+      <c r="H7" s="48">
+        <v>8</v>
+      </c>
+      <c r="I7" s="49">
+        <v>0</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N7" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" s="41">
+        <v>36</v>
+      </c>
+      <c r="P7" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>6</v>
+      </c>
+      <c r="R7" s="48">
+        <v>7</v>
+      </c>
+      <c r="S7" s="49">
+        <v>0</v>
+      </c>
+      <c r="T7" s="48">
+        <v>8</v>
+      </c>
+      <c r="U7" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B8" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="41">
+        <v>40</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="43">
+        <v>8</v>
+      </c>
+      <c r="F8" s="48">
+        <v>9</v>
+      </c>
+      <c r="G8" s="49">
+        <v>0</v>
+      </c>
+      <c r="H8" s="48">
+        <v>10</v>
+      </c>
+      <c r="I8" s="49">
+        <v>0</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="41">
+        <v>40</v>
+      </c>
+      <c r="P8" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q8" s="43">
+        <v>8</v>
+      </c>
+      <c r="R8" s="48">
+        <v>9</v>
+      </c>
+      <c r="S8" s="49">
+        <v>0</v>
+      </c>
+      <c r="T8" s="48">
+        <v>10</v>
+      </c>
+      <c r="U8" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B9" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="41">
+        <v>30</v>
+      </c>
+      <c r="D9" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E9" s="43">
+        <v>5</v>
+      </c>
+      <c r="F9" s="48">
+        <v>6</v>
+      </c>
+      <c r="G9" s="49">
+        <v>0</v>
+      </c>
+      <c r="H9" s="48">
+        <v>6</v>
+      </c>
+      <c r="I9" s="49">
+        <v>0</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="41">
+        <v>30</v>
+      </c>
+      <c r="P9" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q9" s="43">
+        <v>5</v>
+      </c>
+      <c r="R9" s="48">
+        <v>6</v>
+      </c>
+      <c r="S9" s="49">
+        <v>0</v>
+      </c>
+      <c r="T9" s="48">
+        <v>6</v>
+      </c>
+      <c r="U9" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B10" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="41">
+        <v>27</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0.1111</v>
+      </c>
+      <c r="E10" s="43">
+        <v>3</v>
+      </c>
+      <c r="F10" s="48">
+        <v>5</v>
+      </c>
+      <c r="G10" s="49">
+        <v>0</v>
+      </c>
+      <c r="H10" s="48">
+        <v>5</v>
+      </c>
+      <c r="I10" s="49">
+        <v>0</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" s="41">
+        <v>27</v>
+      </c>
+      <c r="P10" s="41">
+        <v>0.1111</v>
+      </c>
+      <c r="Q10" s="43">
+        <v>3</v>
+      </c>
+      <c r="R10" s="48">
+        <v>5</v>
+      </c>
+      <c r="S10" s="49">
+        <v>0</v>
+      </c>
+      <c r="T10" s="48">
+        <v>5</v>
+      </c>
+      <c r="U10" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B11" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="41">
+        <v>24</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0.125</v>
+      </c>
+      <c r="E11" s="43">
+        <v>3</v>
+      </c>
+      <c r="F11" s="48">
+        <v>4</v>
+      </c>
+      <c r="G11" s="49">
+        <v>0</v>
+      </c>
+      <c r="H11" s="48">
+        <v>5</v>
+      </c>
+      <c r="I11" s="49">
+        <v>0</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N11" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="41">
+        <v>24</v>
+      </c>
+      <c r="P11" s="41">
+        <v>0.125</v>
+      </c>
+      <c r="Q11" s="43">
+        <v>3</v>
+      </c>
+      <c r="R11" s="48">
+        <v>4</v>
+      </c>
+      <c r="S11" s="49">
+        <v>0</v>
+      </c>
+      <c r="T11" s="48">
+        <v>5</v>
+      </c>
+      <c r="U11" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B12" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="41">
+        <v>36</v>
+      </c>
+      <c r="D12" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E12" s="43">
+        <v>6</v>
+      </c>
+      <c r="F12" s="48">
+        <v>8</v>
+      </c>
+      <c r="G12" s="49">
+        <v>0</v>
+      </c>
+      <c r="H12" s="48">
+        <v>8</v>
+      </c>
+      <c r="I12" s="49">
+        <v>0</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="L12" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N12" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="O12" s="41">
+        <v>36</v>
+      </c>
+      <c r="P12" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q12" s="43">
+        <v>6</v>
+      </c>
+      <c r="R12" s="48">
+        <v>8</v>
+      </c>
+      <c r="S12" s="49">
+        <v>0</v>
+      </c>
+      <c r="T12" s="48">
+        <v>8</v>
+      </c>
+      <c r="U12" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B13" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="41">
+        <v>35</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="43">
+        <v>7</v>
+      </c>
+      <c r="F13" s="48">
+        <v>8</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0</v>
+      </c>
+      <c r="H13" s="48">
+        <v>9</v>
+      </c>
+      <c r="I13" s="49">
+        <v>0</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N13" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="O13" s="41">
+        <v>35</v>
+      </c>
+      <c r="P13" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q13" s="43">
+        <v>7</v>
+      </c>
+      <c r="R13" s="48">
+        <v>8</v>
+      </c>
+      <c r="S13" s="49">
+        <v>0</v>
+      </c>
+      <c r="T13" s="48">
+        <v>9</v>
+      </c>
+      <c r="U13" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B14" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="41">
+        <v>35</v>
+      </c>
+      <c r="D14" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="43">
+        <v>7</v>
+      </c>
+      <c r="F14" s="48">
+        <v>8</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0</v>
+      </c>
+      <c r="H14" s="48">
+        <v>9</v>
+      </c>
+      <c r="I14" s="49">
+        <v>0</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="41">
+        <v>35</v>
+      </c>
+      <c r="P14" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q14" s="43">
+        <v>7</v>
+      </c>
+      <c r="R14" s="48">
+        <v>8</v>
+      </c>
+      <c r="S14" s="49">
+        <v>0</v>
+      </c>
+      <c r="T14" s="48">
+        <v>9</v>
+      </c>
+      <c r="U14" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B15" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="41">
+        <v>35</v>
+      </c>
+      <c r="D15" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="43">
+        <v>7</v>
+      </c>
+      <c r="F15" s="48">
+        <v>9</v>
+      </c>
+      <c r="G15" s="49">
+        <v>4</v>
+      </c>
+      <c r="H15" s="48">
+        <v>8</v>
+      </c>
+      <c r="I15" s="49">
+        <v>4</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="41">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N15" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="41">
+        <v>35</v>
+      </c>
+      <c r="P15" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q15" s="43">
+        <v>7</v>
+      </c>
+      <c r="R15" s="48">
+        <v>9</v>
+      </c>
+      <c r="S15" s="49">
+        <v>4</v>
+      </c>
+      <c r="T15" s="48">
+        <v>8</v>
+      </c>
+      <c r="U15" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.15">
+      <c r="B16" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="41">
+        <v>25</v>
+      </c>
+      <c r="D16" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="43">
+        <v>5</v>
+      </c>
+      <c r="F16" s="48">
+        <v>7</v>
+      </c>
+      <c r="G16" s="49">
+        <v>1</v>
+      </c>
+      <c r="H16" s="48">
+        <v>6</v>
+      </c>
+      <c r="I16" s="49">
+        <v>1</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="41">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N16" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="O16" s="41">
+        <v>25</v>
+      </c>
+      <c r="P16" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q16" s="43">
+        <v>5</v>
+      </c>
+      <c r="R16" s="48">
+        <v>7</v>
+      </c>
+      <c r="S16" s="49">
+        <v>1</v>
+      </c>
+      <c r="T16" s="48">
+        <v>6</v>
+      </c>
+      <c r="U16" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B17" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="41">
+        <v>25</v>
+      </c>
+      <c r="D17" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="43">
+        <v>5</v>
+      </c>
+      <c r="F17" s="48">
+        <v>7</v>
+      </c>
+      <c r="G17" s="49">
+        <v>1</v>
+      </c>
+      <c r="H17" s="48">
+        <v>6</v>
+      </c>
+      <c r="I17" s="49">
+        <v>1</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="41">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N17" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="O17" s="41">
+        <v>25</v>
+      </c>
+      <c r="P17" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q17" s="43">
+        <v>5</v>
+      </c>
+      <c r="R17" s="48">
+        <v>7</v>
+      </c>
+      <c r="S17" s="49">
+        <v>1</v>
+      </c>
+      <c r="T17" s="48">
+        <v>6</v>
+      </c>
+      <c r="U17" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B18" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="41">
+        <v>30</v>
+      </c>
+      <c r="D18" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E18" s="43">
+        <v>5</v>
+      </c>
+      <c r="F18" s="48">
+        <v>6</v>
+      </c>
+      <c r="G18" s="49">
+        <v>0</v>
+      </c>
+      <c r="H18" s="48">
+        <v>7</v>
+      </c>
+      <c r="I18" s="49">
+        <v>0</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="O18" s="41">
+        <v>30</v>
+      </c>
+      <c r="P18" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q18" s="43">
+        <v>5</v>
+      </c>
+      <c r="R18" s="48">
+        <v>6</v>
+      </c>
+      <c r="S18" s="49">
+        <v>0</v>
+      </c>
+      <c r="T18" s="48">
+        <v>7</v>
+      </c>
+      <c r="U18" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B19" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="41">
+        <v>30</v>
+      </c>
+      <c r="D19" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E19" s="43">
+        <v>5</v>
+      </c>
+      <c r="F19" s="48">
+        <v>6</v>
+      </c>
+      <c r="G19" s="49">
+        <v>0</v>
+      </c>
+      <c r="H19" s="48">
+        <v>7</v>
+      </c>
+      <c r="I19" s="49">
+        <v>0</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="N19" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" s="41">
+        <v>30</v>
+      </c>
+      <c r="P19" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q19" s="43">
+        <v>5</v>
+      </c>
+      <c r="R19" s="48">
+        <v>6</v>
+      </c>
+      <c r="S19" s="49">
+        <v>0</v>
+      </c>
+      <c r="T19" s="48">
+        <v>7</v>
+      </c>
+      <c r="U19" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B20" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="41">
+        <v>25</v>
+      </c>
+      <c r="D20" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="43">
+        <v>5</v>
+      </c>
+      <c r="F20" s="48">
+        <v>7</v>
+      </c>
+      <c r="G20" s="49">
+        <v>2</v>
+      </c>
+      <c r="H20" s="48">
+        <v>6</v>
+      </c>
+      <c r="I20" s="49">
+        <v>2</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="41">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20" s="41">
+        <v>25</v>
+      </c>
+      <c r="P20" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q20" s="43">
+        <v>5</v>
+      </c>
+      <c r="R20" s="48">
+        <v>7</v>
+      </c>
+      <c r="S20" s="49">
+        <v>2</v>
+      </c>
+      <c r="T20" s="48">
+        <v>6</v>
+      </c>
+      <c r="U20" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B21" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="41">
+        <v>25</v>
+      </c>
+      <c r="D21" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="43">
+        <v>5</v>
+      </c>
+      <c r="F21" s="48">
+        <v>6</v>
+      </c>
+      <c r="G21" s="49">
+        <v>1</v>
+      </c>
+      <c r="H21" s="48">
+        <v>6</v>
+      </c>
+      <c r="I21" s="49">
+        <v>1</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="L21" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N21" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21" s="41">
+        <v>25</v>
+      </c>
+      <c r="P21" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q21" s="43">
+        <v>5</v>
+      </c>
+      <c r="R21" s="48">
+        <v>6</v>
+      </c>
+      <c r="S21" s="49">
+        <v>1</v>
+      </c>
+      <c r="T21" s="48">
+        <v>6</v>
+      </c>
+      <c r="U21" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B22" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="41">
+        <v>30</v>
+      </c>
+      <c r="D22" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="E22" s="43">
+        <v>5</v>
+      </c>
+      <c r="F22" s="48">
+        <v>7</v>
+      </c>
+      <c r="G22" s="49">
+        <v>0</v>
+      </c>
+      <c r="H22" s="48">
+        <v>7</v>
+      </c>
+      <c r="I22" s="49">
+        <v>0</v>
+      </c>
+      <c r="K22" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="L22" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>Igual</v>
+      </c>
+      <c r="N22" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="O22" s="41">
+        <v>30</v>
+      </c>
+      <c r="P22" s="41">
+        <v>0.1666</v>
+      </c>
+      <c r="Q22" s="43">
+        <v>5</v>
+      </c>
+      <c r="R22" s="48">
+        <v>7</v>
+      </c>
+      <c r="S22" s="49">
+        <v>0</v>
+      </c>
+      <c r="T22" s="48">
+        <v>7</v>
+      </c>
+      <c r="U22" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="41">
+        <v>25</v>
+      </c>
+      <c r="D23" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="43">
+        <v>5</v>
+      </c>
+      <c r="F23" s="50">
+        <v>7</v>
+      </c>
+      <c r="G23" s="51">
+        <v>0</v>
+      </c>
+      <c r="H23" s="50">
+        <v>6</v>
+      </c>
+      <c r="I23" s="51">
+        <v>0</v>
+      </c>
+      <c r="K23" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="L23" s="41">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N23" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="O23" s="41">
+        <v>25</v>
+      </c>
+      <c r="P23" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="Q23" s="43">
+        <v>5</v>
+      </c>
+      <c r="R23" s="50">
+        <v>7</v>
+      </c>
+      <c r="S23" s="51">
+        <v>0</v>
+      </c>
+      <c r="T23" s="50">
+        <v>6</v>
+      </c>
+      <c r="U23" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" ht="63" x14ac:dyDescent="0.15">
+      <c r="X25" s="40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X26" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X27" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X28" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X29" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X30" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X31" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X32" s="41">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="W33" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="X33" s="41">
+        <f>SUBTOTAL(3,X26:X32)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X34" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="35" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X35" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="36" spans="23:24" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.15">
+      <c r="X36" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="37" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X37" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="38" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X38" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="39" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X39" s="41">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="40" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="W40" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="X40" s="41">
+        <f>SUBTOTAL(3,X34:X39)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X41" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X42" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="23:24" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.15">
+      <c r="X43" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X44" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X45" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X46" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="X47" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="W48" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="X48" s="52">
+        <f>SUBTOTAL(3,X41:X47)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15">
+      <c r="W49" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="X49" s="52">
+        <f>SUBTOTAL(3,X26:X47)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="23:24" hidden="1" outlineLevel="2" x14ac:dyDescent="0.15"/>
+    <row r="51" spans="23:24" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <sortState ref="X26:X45">
+    <sortCondition ref="X29:X48"/>
+  </sortState>
+  <dataConsolidate topLabels="1"/>
+  <mergeCells count="12">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>190</v>
-      </c>
-      <c r="B1">
-        <v>19</v>
-      </c>
-      <c r="C1">
-        <v>8</v>
-      </c>
-      <c r="D1">
-        <v>8</v>
-      </c>
-      <c r="E1">
-        <v>8</v>
-      </c>
-      <c r="H1">
-        <f>SUM(A1:G1)</f>
-        <v>233</v>
-      </c>
-      <c r="I1">
-        <f>233-H1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>79</v>
-      </c>
-      <c r="B2">
-        <v>79</v>
-      </c>
-      <c r="C2">
-        <v>69</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H7" si="0">SUM(A2:G2)</f>
-        <v>233</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I7" si="1">233-H2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>79</v>
-      </c>
-      <c r="B3">
-        <v>79</v>
-      </c>
-      <c r="C3">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H4" si="2">SUM(A3:G3)</f>
-        <v>233</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>79</v>
-      </c>
-      <c r="B4">
-        <v>79</v>
-      </c>
-      <c r="C4">
-        <v>69</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
-        <v>233</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>78</v>
-      </c>
-      <c r="B5">
-        <v>77</v>
-      </c>
-      <c r="C5">
-        <v>76</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>233</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>75</v>
-      </c>
-      <c r="B6">
-        <v>73</v>
-      </c>
-      <c r="C6">
-        <v>71</v>
-      </c>
-      <c r="G6">
-        <v>14</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>233</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>44</v>
-      </c>
-      <c r="C7">
-        <v>36</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="F7">
-        <v>35</v>
-      </c>
-      <c r="G7">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>233</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="2" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="34"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="34"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="34"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="34"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="34"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="34"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="34"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización de documento, ajuste pag web para mostrar contenedores en 2 columnas, ajuste en el almacenamiento de resultados en programa hiperheuristicas
</commit_message>
<xml_diff>
--- a/doc/cuadros y figuras.xlsx
+++ b/doc/cuadros y figuras.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="123">
   <si>
     <t>Instancia 1</t>
   </si>
@@ -382,7 +382,10 @@
     <t>Grand Count</t>
   </si>
   <si>
-    <t>Heurística seleccionada por HH</t>
+    <t>Mejores resultados obtenidos con Heurística:</t>
+  </si>
+  <si>
+    <t>Heurística seleccionada por HH:</t>
   </si>
 </sst>
 </file>
@@ -762,9 +765,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -806,9 +806,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -827,16 +824,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,34 +1156,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -1297,34 +1300,34 @@
       <c r="F9" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -1527,34 +1530,34 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1751,34 +1754,34 @@
       <c r="F37" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
@@ -1971,24 +1974,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" s="21" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -2108,21 +2111,21 @@
       <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -2230,18 +2233,18 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
     </row>
     <row r="26" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
@@ -2508,18 +2511,18 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
     </row>
     <row r="53" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
@@ -2701,18 +2704,18 @@
       <c r="C69" s="17"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="49"/>
-      <c r="C70" s="49"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="47"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="50" t="s">
+      <c r="A71" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="50"/>
-      <c r="C71" s="50"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
     </row>
     <row r="72" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
@@ -2803,18 +2806,18 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="49" t="s">
+      <c r="A81" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="B81" s="49"/>
-      <c r="C81" s="49"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="47"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="50" t="s">
+      <c r="A82" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="48"/>
     </row>
     <row r="83" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
@@ -2942,36 +2945,36 @@
   <dimension ref="B1:Y51"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L23"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="31"/>
-    <col min="2" max="2" width="7.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="32" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="31"/>
-    <col min="12" max="12" width="13" style="32" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="31"/>
-    <col min="14" max="14" width="4.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="9.140625" style="30"/>
+    <col min="2" max="2" width="7.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="31" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="30"/>
+    <col min="12" max="12" width="13" style="31" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="30"/>
+    <col min="14" max="14" width="4.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="11.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:21" s="29" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" s="28" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
         <v>82</v>
       </c>
@@ -2984,15 +2987,15 @@
       <c r="E2" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="53" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="L2" s="30"/>
+      <c r="I2" s="50"/>
+      <c r="L2" s="29"/>
       <c r="N2" s="51" t="s">
         <v>111</v>
       </c>
@@ -3005,1332 +3008,1332 @@
       <c r="Q2" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="R2" s="53" t="s">
+      <c r="R2" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="53" t="s">
+      <c r="S2" s="50"/>
+      <c r="T2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="54"/>
-    </row>
-    <row r="3" spans="2:21" s="29" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="U2" s="50"/>
+    </row>
+    <row r="3" spans="2:21" s="28" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="52"/>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="L3" s="33" t="s">
-        <v>110</v>
+      <c r="L3" s="32" t="s">
+        <v>121</v>
       </c>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="52"/>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="S3" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U3" s="37" t="s">
+      <c r="U3" s="36" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <v>8</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <v>0.5</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="34">
         <v>4</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <v>4</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="38">
         <v>2</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="37">
         <v>4</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="38">
         <v>2</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="34" t="str">
+      <c r="L4" s="33" t="str">
         <f>IF(F4&gt;H4,"DJD 1/4",IF(H4&gt;F4, "DJD 1/3", IF(H4=F4, "Igual")))</f>
         <v>Igual</v>
       </c>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="33">
         <v>8</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="33">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="35">
+      <c r="Q4" s="34">
         <v>4</v>
       </c>
-      <c r="R4" s="38">
+      <c r="R4" s="37">
         <v>4</v>
       </c>
-      <c r="S4" s="39">
+      <c r="S4" s="38">
         <v>2</v>
       </c>
-      <c r="T4" s="38">
+      <c r="T4" s="37">
         <v>4</v>
       </c>
-      <c r="U4" s="39">
+      <c r="U4" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="33">
         <v>30</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="33">
         <v>0.2</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="34">
         <v>6</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="37">
         <v>8</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="38">
         <v>2</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="37">
         <v>7</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="38">
         <v>2</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="34" t="str">
+      <c r="L5" s="33" t="str">
         <f t="shared" ref="L5:L23" si="0">IF(F5&gt;H5,"DJD 1/4",IF(H5&gt;F5, "DJD 1/3", IF(H5=F5, "Igual")))</f>
         <v>DJD 1/4</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="33">
         <v>30</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="34">
         <v>6</v>
       </c>
-      <c r="R5" s="38">
+      <c r="R5" s="37">
         <v>8</v>
       </c>
-      <c r="S5" s="39">
+      <c r="S5" s="38">
         <v>2</v>
       </c>
-      <c r="T5" s="38">
+      <c r="T5" s="37">
         <v>7</v>
       </c>
-      <c r="U5" s="39">
+      <c r="U5" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>28</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>0.25</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <v>7</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="37">
         <v>8</v>
       </c>
-      <c r="G6" s="39">
-        <v>0</v>
-      </c>
-      <c r="H6" s="38">
+      <c r="G6" s="38">
+        <v>0</v>
+      </c>
+      <c r="H6" s="37">
         <v>8</v>
       </c>
-      <c r="I6" s="39">
-        <v>0</v>
-      </c>
-      <c r="K6" s="34" t="s">
+      <c r="I6" s="38">
+        <v>0</v>
+      </c>
+      <c r="K6" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="34" t="str">
+      <c r="L6" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="N6" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="33">
         <v>28</v>
       </c>
-      <c r="P6" s="34">
+      <c r="P6" s="33">
         <v>0.25</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="34">
         <v>7</v>
       </c>
-      <c r="R6" s="38">
+      <c r="R6" s="37">
         <v>8</v>
       </c>
-      <c r="S6" s="39">
-        <v>0</v>
-      </c>
-      <c r="T6" s="38">
+      <c r="S6" s="38">
+        <v>0</v>
+      </c>
+      <c r="T6" s="37">
         <v>8</v>
       </c>
-      <c r="U6" s="39">
+      <c r="U6" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>36</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="34">
         <v>6</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="37">
         <v>7</v>
       </c>
-      <c r="G7" s="39">
-        <v>0</v>
-      </c>
-      <c r="H7" s="38">
+      <c r="G7" s="38">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37">
         <v>8</v>
       </c>
-      <c r="I7" s="39">
-        <v>0</v>
-      </c>
-      <c r="K7" s="34" t="s">
+      <c r="I7" s="38">
+        <v>0</v>
+      </c>
+      <c r="K7" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="34" t="str">
+      <c r="L7" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="N7" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="O7" s="34">
+      <c r="O7" s="33">
         <v>36</v>
       </c>
-      <c r="P7" s="34">
+      <c r="P7" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="34">
         <v>6</v>
       </c>
-      <c r="R7" s="38">
+      <c r="R7" s="37">
         <v>7</v>
       </c>
-      <c r="S7" s="39">
-        <v>0</v>
-      </c>
-      <c r="T7" s="38">
+      <c r="S7" s="38">
+        <v>0</v>
+      </c>
+      <c r="T7" s="37">
         <v>8</v>
       </c>
-      <c r="U7" s="39">
+      <c r="U7" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="33">
         <v>40</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <v>0.2</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="34">
         <v>8</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="37">
         <v>9</v>
       </c>
-      <c r="G8" s="39">
-        <v>0</v>
-      </c>
-      <c r="H8" s="38">
+      <c r="G8" s="38">
+        <v>0</v>
+      </c>
+      <c r="H8" s="37">
         <v>10</v>
       </c>
-      <c r="I8" s="39">
-        <v>0</v>
-      </c>
-      <c r="K8" s="34" t="s">
+      <c r="I8" s="38">
+        <v>0</v>
+      </c>
+      <c r="K8" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="34" t="str">
+      <c r="L8" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="N8" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="33">
         <v>40</v>
       </c>
-      <c r="P8" s="34">
+      <c r="P8" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="34">
         <v>8</v>
       </c>
-      <c r="R8" s="38">
+      <c r="R8" s="37">
         <v>9</v>
       </c>
-      <c r="S8" s="39">
-        <v>0</v>
-      </c>
-      <c r="T8" s="38">
+      <c r="S8" s="38">
+        <v>0</v>
+      </c>
+      <c r="T8" s="37">
         <v>10</v>
       </c>
-      <c r="U8" s="39">
+      <c r="U8" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="33">
         <v>30</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="34">
         <v>5</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="37">
         <v>6</v>
       </c>
-      <c r="G9" s="39">
-        <v>0</v>
-      </c>
-      <c r="H9" s="38">
+      <c r="G9" s="38">
+        <v>0</v>
+      </c>
+      <c r="H9" s="37">
         <v>6</v>
       </c>
-      <c r="I9" s="39">
-        <v>0</v>
-      </c>
-      <c r="K9" s="34" t="s">
+      <c r="I9" s="38">
+        <v>0</v>
+      </c>
+      <c r="K9" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="L9" s="34" t="str">
+      <c r="L9" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="N9" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="33">
         <v>30</v>
       </c>
-      <c r="P9" s="34">
+      <c r="P9" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="34">
         <v>5</v>
       </c>
-      <c r="R9" s="38">
+      <c r="R9" s="37">
         <v>6</v>
       </c>
-      <c r="S9" s="39">
-        <v>0</v>
-      </c>
-      <c r="T9" s="38">
+      <c r="S9" s="38">
+        <v>0</v>
+      </c>
+      <c r="T9" s="37">
         <v>6</v>
       </c>
-      <c r="U9" s="39">
+      <c r="U9" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="33">
         <v>27</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="33">
         <v>0.1111</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="34">
         <v>3</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>5</v>
       </c>
-      <c r="G10" s="39">
-        <v>0</v>
-      </c>
-      <c r="H10" s="38">
+      <c r="G10" s="38">
+        <v>0</v>
+      </c>
+      <c r="H10" s="37">
         <v>5</v>
       </c>
-      <c r="I10" s="39">
-        <v>0</v>
-      </c>
-      <c r="K10" s="34" t="s">
+      <c r="I10" s="38">
+        <v>0</v>
+      </c>
+      <c r="K10" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="L10" s="34" t="str">
+      <c r="L10" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N10" s="34" t="s">
+      <c r="N10" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="33">
         <v>27</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="33">
         <v>0.1111</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="34">
         <v>3</v>
       </c>
-      <c r="R10" s="38">
+      <c r="R10" s="37">
         <v>5</v>
       </c>
-      <c r="S10" s="39">
-        <v>0</v>
-      </c>
-      <c r="T10" s="38">
+      <c r="S10" s="38">
+        <v>0</v>
+      </c>
+      <c r="T10" s="37">
         <v>5</v>
       </c>
-      <c r="U10" s="39">
+      <c r="U10" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="33">
         <v>24</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="33">
         <v>0.125</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <v>3</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="37">
         <v>4</v>
       </c>
-      <c r="G11" s="39">
-        <v>0</v>
-      </c>
-      <c r="H11" s="38">
+      <c r="G11" s="38">
+        <v>0</v>
+      </c>
+      <c r="H11" s="37">
         <v>5</v>
       </c>
-      <c r="I11" s="39">
-        <v>0</v>
-      </c>
-      <c r="K11" s="34" t="s">
+      <c r="I11" s="38">
+        <v>0</v>
+      </c>
+      <c r="K11" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="L11" s="34" t="str">
+      <c r="L11" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N11" s="34" t="s">
+      <c r="N11" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="33">
         <v>24</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="33">
         <v>0.125</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="Q11" s="34">
         <v>3</v>
       </c>
-      <c r="R11" s="38">
+      <c r="R11" s="37">
         <v>4</v>
       </c>
-      <c r="S11" s="39">
-        <v>0</v>
-      </c>
-      <c r="T11" s="38">
+      <c r="S11" s="38">
+        <v>0</v>
+      </c>
+      <c r="T11" s="37">
         <v>5</v>
       </c>
-      <c r="U11" s="39">
+      <c r="U11" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="33">
         <v>36</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="34">
         <v>6</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="37">
         <v>8</v>
       </c>
-      <c r="G12" s="39">
-        <v>0</v>
-      </c>
-      <c r="H12" s="38">
+      <c r="G12" s="38">
+        <v>0</v>
+      </c>
+      <c r="H12" s="37">
         <v>8</v>
       </c>
-      <c r="I12" s="39">
-        <v>0</v>
-      </c>
-      <c r="K12" s="34" t="s">
+      <c r="I12" s="38">
+        <v>0</v>
+      </c>
+      <c r="K12" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="34" t="str">
+      <c r="L12" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="34">
+      <c r="O12" s="33">
         <v>36</v>
       </c>
-      <c r="P12" s="34">
+      <c r="P12" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="34">
         <v>6</v>
       </c>
-      <c r="R12" s="38">
+      <c r="R12" s="37">
         <v>8</v>
       </c>
-      <c r="S12" s="39">
-        <v>0</v>
-      </c>
-      <c r="T12" s="38">
+      <c r="S12" s="38">
+        <v>0</v>
+      </c>
+      <c r="T12" s="37">
         <v>8</v>
       </c>
-      <c r="U12" s="39">
+      <c r="U12" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <v>35</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="33">
         <v>0.2</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <v>7</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="37">
         <v>8</v>
       </c>
-      <c r="G13" s="39">
-        <v>0</v>
-      </c>
-      <c r="H13" s="38">
+      <c r="G13" s="38">
+        <v>0</v>
+      </c>
+      <c r="H13" s="37">
         <v>9</v>
       </c>
-      <c r="I13" s="39">
-        <v>0</v>
-      </c>
-      <c r="K13" s="34" t="s">
+      <c r="I13" s="38">
+        <v>0</v>
+      </c>
+      <c r="K13" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="34" t="str">
+      <c r="L13" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="N13" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="33">
         <v>35</v>
       </c>
-      <c r="P13" s="34">
+      <c r="P13" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="34">
         <v>7</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="37">
         <v>8</v>
       </c>
-      <c r="S13" s="39">
-        <v>0</v>
-      </c>
-      <c r="T13" s="38">
+      <c r="S13" s="38">
+        <v>0</v>
+      </c>
+      <c r="T13" s="37">
         <v>9</v>
       </c>
-      <c r="U13" s="39">
+      <c r="U13" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <v>35</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="33">
         <v>0.2</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="34">
         <v>7</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="37">
         <v>8</v>
       </c>
-      <c r="G14" s="39">
-        <v>0</v>
-      </c>
-      <c r="H14" s="38">
+      <c r="G14" s="38">
+        <v>0</v>
+      </c>
+      <c r="H14" s="37">
         <v>9</v>
       </c>
-      <c r="I14" s="39">
-        <v>0</v>
-      </c>
-      <c r="K14" s="34" t="s">
+      <c r="I14" s="38">
+        <v>0</v>
+      </c>
+      <c r="K14" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="34" t="str">
+      <c r="L14" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N14" s="34" t="s">
+      <c r="N14" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="O14" s="34">
+      <c r="O14" s="33">
         <v>35</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P14" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="34">
         <v>7</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="37">
         <v>8</v>
       </c>
-      <c r="S14" s="39">
-        <v>0</v>
-      </c>
-      <c r="T14" s="38">
+      <c r="S14" s="38">
+        <v>0</v>
+      </c>
+      <c r="T14" s="37">
         <v>9</v>
       </c>
-      <c r="U14" s="39">
+      <c r="U14" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <v>35</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="33">
         <v>0.2</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="34">
         <v>7</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="37">
         <v>9</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="38">
         <v>4</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="37">
         <v>8</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="38">
         <v>4</v>
       </c>
-      <c r="K15" s="34" t="s">
+      <c r="K15" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="34" t="str">
+      <c r="L15" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/4</v>
       </c>
-      <c r="N15" s="34" t="s">
+      <c r="N15" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="33">
         <v>35</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="34">
         <v>7</v>
       </c>
-      <c r="R15" s="38">
+      <c r="R15" s="37">
         <v>9</v>
       </c>
-      <c r="S15" s="39">
+      <c r="S15" s="38">
         <v>4</v>
       </c>
-      <c r="T15" s="38">
+      <c r="T15" s="37">
         <v>8</v>
       </c>
-      <c r="U15" s="39">
+      <c r="U15" s="38">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.15">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <v>25</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="33">
         <v>0.2</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="34">
         <v>5</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="37">
         <v>7</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="38">
         <v>1</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="37">
         <v>6</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="38">
         <v>1</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="34" t="str">
+      <c r="L16" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/4</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="33">
         <v>25</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="34">
         <v>5</v>
       </c>
-      <c r="R16" s="38">
+      <c r="R16" s="37">
         <v>7</v>
       </c>
-      <c r="S16" s="39">
+      <c r="S16" s="38">
         <v>1</v>
       </c>
-      <c r="T16" s="38">
+      <c r="T16" s="37">
         <v>6</v>
       </c>
-      <c r="U16" s="39">
+      <c r="U16" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <v>25</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <v>0.2</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="34">
         <v>5</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="37">
         <v>7</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="38">
         <v>1</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="37">
         <v>6</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="38">
         <v>1</v>
       </c>
-      <c r="K17" s="34" t="s">
+      <c r="K17" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="L17" s="34" t="str">
+      <c r="L17" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/4</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="33">
         <v>25</v>
       </c>
-      <c r="P17" s="34">
+      <c r="P17" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="34">
         <v>5</v>
       </c>
-      <c r="R17" s="38">
+      <c r="R17" s="37">
         <v>7</v>
       </c>
-      <c r="S17" s="39">
+      <c r="S17" s="38">
         <v>1</v>
       </c>
-      <c r="T17" s="38">
+      <c r="T17" s="37">
         <v>6</v>
       </c>
-      <c r="U17" s="39">
+      <c r="U17" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <v>30</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="34">
         <v>5</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="37">
         <v>6</v>
       </c>
-      <c r="G18" s="39">
-        <v>0</v>
-      </c>
-      <c r="H18" s="38">
+      <c r="G18" s="38">
+        <v>0</v>
+      </c>
+      <c r="H18" s="37">
         <v>7</v>
       </c>
-      <c r="I18" s="39">
-        <v>0</v>
-      </c>
-      <c r="K18" s="34" t="s">
+      <c r="I18" s="38">
+        <v>0</v>
+      </c>
+      <c r="K18" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="L18" s="34" t="str">
+      <c r="L18" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="O18" s="34">
+      <c r="O18" s="33">
         <v>30</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="34">
         <v>5</v>
       </c>
-      <c r="R18" s="38">
+      <c r="R18" s="37">
         <v>6</v>
       </c>
-      <c r="S18" s="39">
-        <v>0</v>
-      </c>
-      <c r="T18" s="38">
+      <c r="S18" s="38">
+        <v>0</v>
+      </c>
+      <c r="T18" s="37">
         <v>7</v>
       </c>
-      <c r="U18" s="39">
+      <c r="U18" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="33">
         <v>30</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="34">
         <v>5</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="37">
         <v>6</v>
       </c>
-      <c r="G19" s="39">
-        <v>0</v>
-      </c>
-      <c r="H19" s="38">
+      <c r="G19" s="38">
+        <v>0</v>
+      </c>
+      <c r="H19" s="37">
         <v>7</v>
       </c>
-      <c r="I19" s="39">
-        <v>0</v>
-      </c>
-      <c r="K19" s="34" t="s">
+      <c r="I19" s="38">
+        <v>0</v>
+      </c>
+      <c r="K19" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="34" t="str">
+      <c r="L19" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/3</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="O19" s="34">
+      <c r="O19" s="33">
         <v>30</v>
       </c>
-      <c r="P19" s="34">
+      <c r="P19" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="34">
         <v>5</v>
       </c>
-      <c r="R19" s="38">
+      <c r="R19" s="37">
         <v>6</v>
       </c>
-      <c r="S19" s="39">
-        <v>0</v>
-      </c>
-      <c r="T19" s="38">
+      <c r="S19" s="38">
+        <v>0</v>
+      </c>
+      <c r="T19" s="37">
         <v>7</v>
       </c>
-      <c r="U19" s="39">
+      <c r="U19" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <v>25</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="33">
         <v>0.2</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="34">
         <v>5</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="37">
         <v>7</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="38">
         <v>2</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="37">
         <v>6</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="38">
         <v>2</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="L20" s="34" t="str">
+      <c r="L20" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/4</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="N20" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="O20" s="34">
+      <c r="O20" s="33">
         <v>25</v>
       </c>
-      <c r="P20" s="34">
+      <c r="P20" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q20" s="34">
         <v>5</v>
       </c>
-      <c r="R20" s="38">
+      <c r="R20" s="37">
         <v>7</v>
       </c>
-      <c r="S20" s="39">
+      <c r="S20" s="38">
         <v>2</v>
       </c>
-      <c r="T20" s="38">
+      <c r="T20" s="37">
         <v>6</v>
       </c>
-      <c r="U20" s="39">
+      <c r="U20" s="38">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="33">
         <v>25</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="33">
         <v>0.2</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="34">
         <v>5</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="37">
         <v>6</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="38">
         <v>1</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="37">
         <v>6</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="38">
         <v>1</v>
       </c>
-      <c r="K21" s="34" t="s">
+      <c r="K21" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="L21" s="34" t="str">
+      <c r="L21" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N21" s="34" t="s">
+      <c r="N21" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="O21" s="34">
+      <c r="O21" s="33">
         <v>25</v>
       </c>
-      <c r="P21" s="34">
+      <c r="P21" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="34">
         <v>5</v>
       </c>
-      <c r="R21" s="38">
+      <c r="R21" s="37">
         <v>6</v>
       </c>
-      <c r="S21" s="39">
+      <c r="S21" s="38">
         <v>1</v>
       </c>
-      <c r="T21" s="38">
+      <c r="T21" s="37">
         <v>6</v>
       </c>
-      <c r="U21" s="39">
+      <c r="U21" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <v>30</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="33">
         <v>0.1666</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="34">
         <v>5</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="37">
         <v>7</v>
       </c>
-      <c r="G22" s="39">
-        <v>0</v>
-      </c>
-      <c r="H22" s="38">
+      <c r="G22" s="38">
+        <v>0</v>
+      </c>
+      <c r="H22" s="37">
         <v>7</v>
       </c>
-      <c r="I22" s="39">
-        <v>0</v>
-      </c>
-      <c r="K22" s="34" t="s">
+      <c r="I22" s="38">
+        <v>0</v>
+      </c>
+      <c r="K22" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L22" s="34" t="str">
+      <c r="L22" s="33" t="str">
         <f t="shared" si="0"/>
         <v>Igual</v>
       </c>
-      <c r="N22" s="34" t="s">
+      <c r="N22" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="O22" s="34">
+      <c r="O22" s="33">
         <v>30</v>
       </c>
-      <c r="P22" s="34">
+      <c r="P22" s="33">
         <v>0.1666</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="34">
         <v>5</v>
       </c>
-      <c r="R22" s="38">
+      <c r="R22" s="37">
         <v>7</v>
       </c>
-      <c r="S22" s="39">
-        <v>0</v>
-      </c>
-      <c r="T22" s="38">
+      <c r="S22" s="38">
+        <v>0</v>
+      </c>
+      <c r="T22" s="37">
         <v>7</v>
       </c>
-      <c r="U22" s="39">
+      <c r="U22" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:25" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="33">
         <v>25</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="33">
         <v>0.2</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="34">
         <v>5</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="39">
         <v>7</v>
       </c>
-      <c r="G23" s="41">
-        <v>0</v>
-      </c>
-      <c r="H23" s="40">
+      <c r="G23" s="40">
+        <v>0</v>
+      </c>
+      <c r="H23" s="39">
         <v>6</v>
       </c>
-      <c r="I23" s="41">
-        <v>0</v>
-      </c>
-      <c r="K23" s="34" t="s">
+      <c r="I23" s="40">
+        <v>0</v>
+      </c>
+      <c r="K23" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="L23" s="34" t="str">
+      <c r="L23" s="33" t="str">
         <f t="shared" si="0"/>
         <v>DJD 1/4</v>
       </c>
-      <c r="N23" s="34" t="s">
+      <c r="N23" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="O23" s="34">
+      <c r="O23" s="33">
         <v>25</v>
       </c>
-      <c r="P23" s="34">
+      <c r="P23" s="33">
         <v>0.2</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="Q23" s="34">
         <v>5</v>
       </c>
-      <c r="R23" s="40">
+      <c r="R23" s="39">
         <v>7</v>
       </c>
-      <c r="S23" s="41">
-        <v>0</v>
-      </c>
-      <c r="T23" s="40">
+      <c r="S23" s="40">
+        <v>0</v>
+      </c>
+      <c r="T23" s="39">
         <v>6</v>
       </c>
-      <c r="U23" s="41">
+      <c r="U23" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:25" ht="63" x14ac:dyDescent="0.15">
-      <c r="Y25" s="33" t="s">
+      <c r="Y25" s="32" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y26" s="34">
+      <c r="Y26" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y27" s="34">
+      <c r="Y27" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y28" s="34">
+      <c r="Y28" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="29" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y29" s="34">
+      <c r="Y29" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y30" s="34">
+      <c r="Y30" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="2:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y31" s="34">
+      <c r="Y31" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="2:25" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="X32" s="43" t="s">
+      <c r="X32" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="Y32" s="34">
+      <c r="Y32" s="33">
         <f>SUBTOTAL(3,Y26:Y31)</f>
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y33" s="34">
+      <c r="Y33" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="34" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y34" s="34">
+      <c r="Y34" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="35" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y35" s="34">
+      <c r="Y35" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="36" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y36" s="34">
+      <c r="Y36" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="37" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y37" s="34">
+      <c r="Y37" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="38" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y38" s="34">
+      <c r="Y38" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="39" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y39" s="34">
+      <c r="Y39" s="33">
         <v>0.33</v>
       </c>
     </row>
     <row r="40" spans="24:25" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="X40" s="43" t="s">
+      <c r="X40" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="Y40" s="34">
+      <c r="Y40" s="33">
         <f>SUBTOTAL(3,Y33:Y39)</f>
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y41" s="34" t="s">
+      <c r="Y41" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="42" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y42" s="34" t="s">
+      <c r="Y42" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="43" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y43" s="34" t="s">
+      <c r="Y43" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="44" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y44" s="34" t="s">
+      <c r="Y44" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="45" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y45" s="34" t="s">
+      <c r="Y45" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y46" s="34" t="s">
+      <c r="Y46" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="47" spans="24:25" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="Y47" s="34" t="s">
+      <c r="Y47" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="24:25" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="X48" s="43" t="s">
+      <c r="X48" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="Y48" s="42">
+      <c r="Y48" s="41">
         <f>SUBTOTAL(3,Y41:Y47)</f>
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="24:25" x14ac:dyDescent="0.15">
-      <c r="X49" s="43" t="s">
+      <c r="X49" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="Y49" s="42">
+      <c r="Y49" s="41">
         <f>SUBTOTAL(3,Y26:Y47)</f>
         <v>20</v>
       </c>
@@ -4366,205 +4369,246 @@
   <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="17"/>
+    <col min="3" max="4" width="22.7109375" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:4" ht="36" x14ac:dyDescent="0.2">
+      <c r="B2" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="D2" s="54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="28"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="D3" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="D4" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="D5" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="28"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="D6" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="D7" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="D8" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="D9" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="D10" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="D11" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="D12" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="D13" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="D14" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="D15" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="28"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="D16" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="D17" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+      <c r="D18" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="D19" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="28"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="D20" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="28"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="D21" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="18" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>